<commit_message>
Pushing simulation with observer for Ralle
</commit_message>
<xml_diff>
--- a/_ProcessDocuments/TimePlan/TimePlan_00.xlsx
+++ b/_ProcessDocuments/TimePlan/TimePlan_00.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E52436D-8AD0-8342-BF92-EDDE6C556829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D57A272-FC31-40E7-BFEB-A4BCD47B03B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Timeline" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Project Timeline</t>
   </si>
@@ -116,17 +116,22 @@
   <si>
     <t>Officially Project delivery</t>
   </si>
+  <si>
+    <t>PBL day</t>
+  </si>
+  <si>
+    <t>PBL one page deadline</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -302,7 +307,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -393,11 +398,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -411,8 +419,8 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -426,7 +434,7 @@
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="11" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Per cent" xfId="10" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="10" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="7">
@@ -445,7 +453,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="right" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -522,7 +530,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1459,6 +1467,52 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B92B7070-5ECC-4F0C-A510-1BBF68A023B7}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-GB" baseline="0"/>
+                      <a:t>
+</a:t>
+                    </a:r>
+                    <a:fld id="{2C9756D0-F432-4E6C-81A2-71638A9380A9}" type="CATEGORYNAME">
+                      <a:rPr lang="en-GB" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-165C-465C-AA9E-094AB54D9709}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1480,7 +1534,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-DK"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1532,9 +1586,9 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'Project Timeline'!$C$17:$C$33</c:f>
+              <c:f>'Project Timeline'!$C$17:$C$35</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Project Start</c:v>
                 </c:pt>
@@ -1566,24 +1620,30 @@
                   <c:v>Robust controller design</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>PBL day</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Test simulation / benchmark</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
+                  <c:v>PBL one page deadline</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>Project done</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>Officially Project delivery</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>Exam: Optimality</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>Exam: Fault detection</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>Exam: Modelling</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>Exam: project</c:v>
                 </c:pt>
               </c:strCache>
@@ -1591,10 +1651,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Project Timeline'!$E$17:$E$33</c:f>
+              <c:f>'Project Timeline'!$E$17:$E$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1626,24 +1686,30 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>-5</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>-20</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>-15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>-10</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>-5</c:v>
                 </c:pt>
               </c:numCache>
@@ -1652,9 +1718,9 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>'Project Timeline'!$D$17:$D$33</c15:f>
+                <c15:f>'Project Timeline'!$D$17:$D$35</c15:f>
                 <c15:dlblRangeCache>
-                  <c:ptCount val="17"/>
+                  <c:ptCount val="19"/>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
             </c:ext>
@@ -1748,10 +1814,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>'Project Timeline'!$B$17:$B$33</c:f>
+              <c:f>'Project Timeline'!$B$17:$B$35</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>44593</c:v>
                 </c:pt>
@@ -1773,34 +1839,40 @@
                 <c:pt idx="6">
                   <c:v>44668</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="m/d/yyyy">
+                <c:pt idx="7">
                   <c:v>44676</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="m/d/yyyy">
+                <c:pt idx="8">
                   <c:v>44678</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="m/d/yyyy">
+                <c:pt idx="9">
                   <c:v>44686</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="m/d/yyyy">
+                <c:pt idx="10">
+                  <c:v>44691</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>44693</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="m/d/yyyy">
+                <c:pt idx="12">
+                  <c:v>44698</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>44701</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="m/d/yyyy">
+                <c:pt idx="14">
                   <c:v>44706</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="m/d/yyyy">
+                <c:pt idx="15">
                   <c:v>44713</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="m/d/yyyy">
+                <c:pt idx="16">
                   <c:v>44715</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="m/d/yyyy">
+                <c:pt idx="17">
                   <c:v>44722</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="m/d/yyyy">
+                <c:pt idx="18">
                   <c:v>44729</c:v>
                 </c:pt>
               </c:numCache>
@@ -1808,10 +1880,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Project Timeline'!$F$17:$F$37</c:f>
+              <c:f>'Project Timeline'!$F$17:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1867,6 +1939,12 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1928,7 +2006,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="717044496"/>
@@ -2021,7 +2099,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-DK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2520,8 +2598,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ProjectDetails" displayName="ProjectDetails" ref="B16:G35" totalsRowShown="0" headerRowDxfId="4">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B17:F36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ProjectDetails" displayName="ProjectDetails" ref="B16:G37" totalsRowShown="0" headerRowDxfId="4">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B17:F38">
     <sortCondition ref="B21"/>
   </sortState>
   <tableColumns count="6">
@@ -2810,32 +2888,32 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="19" customWidth="1"/>
-    <col min="3" max="3" width="30.5" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="13" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" style="2" customWidth="1"/>
     <col min="8" max="11" width="9.33203125" style="2"/>
     <col min="12" max="12" width="11.6640625" style="2" customWidth="1"/>
     <col min="13" max="16384" width="9.33203125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="23" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="23" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8"/>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
+      <c r="C1" s="34"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2846,178 +2924,178 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
+    <row r="2" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
     </row>
-    <row r="3" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
+    <row r="3" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
     </row>
-    <row r="4" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
+    <row r="4" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
     </row>
-    <row r="5" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
+    <row r="5" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
     </row>
-    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
+    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
     </row>
-    <row r="7" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
+    <row r="7" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
     </row>
-    <row r="8" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
+    <row r="8" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
     </row>
-    <row r="9" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
+    <row r="9" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
     </row>
-    <row r="10" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
+    <row r="10" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
     </row>
-    <row r="11" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
+    <row r="11" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
     </row>
-    <row r="12" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
+    <row r="12" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
     </row>
-    <row r="13" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
+    <row r="13" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
     </row>
-    <row r="14" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
+    <row r="14" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
     </row>
-    <row r="15" spans="1:12" s="25" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" s="25" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
       <c r="B15" s="26" t="s">
         <v>1</v>
@@ -3033,7 +3111,7 @@
       <c r="K15" s="4"/>
       <c r="L15" s="21"/>
     </row>
-    <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="20" t="s">
         <v>2</v>
       </c>
@@ -3052,14 +3130,14 @@
       <c r="G16" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="34" t="s">
+      <c r="H16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="34"/>
+      <c r="I16" s="35"/>
       <c r="J16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="12">
         <v>44593</v>
       </c>
@@ -3074,15 +3152,15 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="H17" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
     </row>
-    <row r="18" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="12">
         <v>44613</v>
       </c>
@@ -3097,13 +3175,13 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
     </row>
-    <row r="19" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <v>44634</v>
       </c>
@@ -3118,13 +3196,13 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
     </row>
-    <row r="20" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="12">
         <v>44641</v>
       </c>
@@ -3139,13 +3217,13 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
     </row>
-    <row r="21" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
         <v>44645</v>
       </c>
@@ -3166,7 +3244,7 @@
       <c r="K21" s="18"/>
       <c r="L21" s="18"/>
     </row>
-    <row r="22" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="12">
         <v>44665</v>
       </c>
@@ -3187,7 +3265,7 @@
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
     </row>
-    <row r="23" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="12">
         <v>44668</v>
       </c>
@@ -3208,8 +3286,8 @@
       <c r="K23" s="18"/>
       <c r="L23" s="18"/>
     </row>
-    <row r="24" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="36">
+    <row r="24" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="32">
         <v>44676</v>
       </c>
       <c r="C24" s="29" t="s">
@@ -3229,8 +3307,8 @@
       <c r="K24" s="18"/>
       <c r="L24" s="18"/>
     </row>
-    <row r="25" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="36">
+    <row r="25" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="32">
         <v>44678</v>
       </c>
       <c r="C25" s="29" t="s">
@@ -3250,7 +3328,7 @@
       <c r="K25" s="18"/>
       <c r="L25" s="18"/>
     </row>
-    <row r="26" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="30">
         <v>44686</v>
       </c>
@@ -3271,83 +3349,91 @@
       <c r="K26" s="18"/>
       <c r="L26" s="18"/>
     </row>
-    <row r="27" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="30">
-        <v>44693</v>
+        <v>44691</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="4">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="F27" s="11">
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
     </row>
-    <row r="28" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="36">
-        <v>44701</v>
+    <row r="28" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="30">
+        <v>44693</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D28" s="28"/>
-      <c r="E28" s="9">
-        <v>15</v>
+      <c r="E28" s="4">
+        <v>10</v>
       </c>
       <c r="F28" s="11">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="I28" s="5"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
     </row>
-    <row r="29" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="36">
-        <v>44706</v>
+    <row r="29" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="30">
+        <v>44698</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D29" s="28"/>
-      <c r="E29" s="9">
-        <v>-5</v>
+      <c r="E29" s="37">
+        <v>-10</v>
       </c>
       <c r="F29" s="11">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="36">
-        <v>44713</v>
+    <row r="30" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="32">
+        <v>44701</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D30" s="28"/>
       <c r="E30" s="9">
-        <v>-20</v>
+        <v>15</v>
       </c>
       <c r="F30" s="11">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H30" s="6"/>
+      <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="36">
-        <v>44715</v>
+    <row r="31" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="32">
+        <v>44706</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D31" s="28"/>
       <c r="E31" s="9">
-        <v>-15</v>
+        <v>-5</v>
       </c>
       <c r="F31" s="11">
         <f>0</f>
@@ -3355,16 +3441,16 @@
       </c>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="36">
-        <v>44722</v>
+    <row r="32" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="32">
+        <v>44713</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D32" s="28"/>
       <c r="E32" s="9">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="F32" s="11">
         <f>0</f>
@@ -3372,16 +3458,16 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="36">
-        <v>44729</v>
+    <row r="33" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="32">
+        <v>44715</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D33" s="28"/>
       <c r="E33" s="9">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="F33" s="11">
         <f>0</f>
@@ -3389,36 +3475,70 @@
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="36"/>
-      <c r="C34" s="29"/>
+    <row r="34" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="32">
+        <v>44722</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>22</v>
+      </c>
       <c r="D34" s="28"/>
-      <c r="E34" s="9"/>
+      <c r="E34" s="9">
+        <v>-10</v>
+      </c>
       <c r="F34" s="11">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H34" s="7"/>
+      <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="30"/>
-      <c r="C35" s="29"/>
+    <row r="35" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="32">
+        <v>44729</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>25</v>
+      </c>
       <c r="D35" s="28"/>
+      <c r="E35" s="9">
+        <v>-5</v>
+      </c>
       <c r="F35" s="11">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="G35" s="7"/>
+      <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="E36" s="2"/>
+    <row r="36" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="32"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="E37" s="2"/>
+    <row r="37" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="30"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="28"/>
+      <c r="F37" s="11">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3460,6 +3580,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9677210f24a1be23c92c90fd886aa0aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e05723c5c1908df1a1a4ebf11d344e" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -3670,14 +3798,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9EFE20-B0BF-4817-AA37-C0305E12107B}">
   <ds:schemaRefs>
@@ -3687,6 +3807,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71E3CE6-3BAB-4EFC-B954-0CB76BF2E2C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F56DC957-990F-47B2-AF0D-7029CF1F606B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3703,14 +3833,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71E3CE6-3BAB-4EFC-B954-0CB76BF2E2C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>